<commit_message>
added updated test data sheet
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\venkata_srinadhuni\git\Selenium_POM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E003613\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E518D699-A3C4-44BF-AB1D-59676E85E2C0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8A4492-60C4-4656-A7E8-85D638358C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login_Test_Case_01" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
     <t>Gmail</t>
   </si>
   <si>
-    <t>Infosys</t>
+    <t>CGI</t>
   </si>
 </sst>
 </file>
@@ -403,33 +403,33 @@
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1796875" customWidth="1"/>
+    <col min="7" max="7" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="28.453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" customWidth="1"/>
+    <col min="14" max="14" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.81640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -437,7 +437,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -463,22 +463,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -497,22 +497,22 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -531,13 +531,13 @@
       <selection activeCell="G5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -545,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -571,13 +571,13 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.54296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -585,7 +585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Uploaded test data file
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\E003613\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8A4492-60C4-4656-A7E8-85D638358C9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24362EC0-9535-410B-9E72-E1EC0D745DAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,9 +46,6 @@
     <t>TextToSearch</t>
   </si>
   <si>
-    <t>LinkedIn</t>
-  </si>
-  <si>
     <t>Username</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
   </si>
   <si>
     <t>CGI</t>
+  </si>
+  <si>
+    <t>Cigniti</t>
   </si>
 </sst>
 </file>
@@ -475,12 +475,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -509,12 +509,12 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +539,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +579,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -587,10 +587,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>